<commit_message>
Final corrections for IW+ v2.2 pre-Usetox3 switch.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei312/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei312/ei_iw_mapping.xlsx
@@ -8,19 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei312\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573A8F07-8F8B-48ED-962E-6E38F7B24C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD93561-E623-47B5-BF90-3337061F811C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$2300</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5401" uniqueCount="2645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2646">
   <si>
     <t>ecoinvent name</t>
   </si>
@@ -7955,6 +7971,9 @@
   </si>
   <si>
     <t>CF from a specific member of the aggregated category taken as proxy</t>
+  </si>
+  <si>
+    <t>Lithium (I)</t>
   </si>
 </sst>
 </file>
@@ -8324,8 +8343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A644" workbookViewId="0">
-      <selection activeCell="A659" sqref="A659"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11032,6 +11051,9 @@
       <c r="A259" t="s">
         <v>261</v>
       </c>
+      <c r="B259" t="s">
+        <v>261</v>
+      </c>
       <c r="C259" t="s">
         <v>2641</v>
       </c>
@@ -19887,6 +19909,9 @@
       <c r="A1133" t="s">
         <v>1135</v>
       </c>
+      <c r="B1133" t="s">
+        <v>1135</v>
+      </c>
       <c r="C1133" t="s">
         <v>2641</v>
       </c>
@@ -24187,6 +24212,9 @@
       <c r="A1579" t="s">
         <v>1581</v>
       </c>
+      <c r="B1579" t="s">
+        <v>2645</v>
+      </c>
       <c r="C1579">
         <v>3.9</v>
       </c>
@@ -25269,6 +25297,9 @@
       <c r="A1700" t="s">
         <v>1702</v>
       </c>
+      <c r="B1700" t="s">
+        <v>1135</v>
+      </c>
       <c r="C1700">
         <v>3.9</v>
       </c>
@@ -31691,6 +31722,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D2300" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>